<commit_message>
v0.0.1: overhaul, folder structure, date in file
</commit_message>
<xml_diff>
--- a/Example_file.xlsx
+++ b/Example_file.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58581D24-5C6C-4696-9E4C-4745B244B607}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABE8CED7-1E14-4952-A602-81C2F83FA76A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -93,7 +93,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -106,8 +106,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -219,11 +225,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -256,6 +299,30 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="2" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -265,29 +332,14 @@
     <xf numFmtId="2" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -572,7 +624,7 @@
   <dimension ref="A1:M68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q12" sqref="Q12"/>
+      <selection activeCell="K1" sqref="K1:M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -590,73 +642,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="16"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="24"/>
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="27"/>
     </row>
     <row r="2" spans="1:13" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="F2" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="22" t="s">
+      <c r="G2" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="22" t="s">
+      <c r="H2" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="22" t="s">
+      <c r="I2" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="22" t="s">
+      <c r="J2" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="22" t="s">
+      <c r="K2" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="22" t="s">
+      <c r="L2" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="24" t="s">
+      <c r="M2" s="21" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:13" s="4" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="17"/>
-      <c r="B3" s="18"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="20"/>
-      <c r="L3" s="20"/>
-      <c r="M3" s="20"/>
+      <c r="A3" s="14"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="17"/>
+      <c r="M3" s="17"/>
     </row>
     <row r="4" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10"/>

</xml_diff>